<commit_message>
Update demo tests & resources
</commit_message>
<xml_diff>
--- a/src/test/resources/product_catalog.xlsx
+++ b/src/test/resources/product_catalog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kapileson/Desktop/jmh-test-playground/src/main/resources/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kapileson/Desktop/jmh-test-playground/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4F8A035-0929-B441-9216-A2DA25BE9C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C863D4-7F60-B244-A204-657CF98B7ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{8743DBB3-9E11-0445-A543-E7BF86D17E3C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Id</t>
   </si>
@@ -74,12 +74,6 @@
     <t>109_</t>
   </si>
   <si>
-    <t>1+11</t>
-  </si>
-  <si>
-    <t>11=2</t>
-  </si>
-  <si>
     <t>Potato_Vegetable</t>
   </si>
   <si>
@@ -87,6 +81,21 @@
   </si>
   <si>
     <t>Products</t>
+  </si>
+  <si>
+    <t>Grapes_Fruit</t>
+  </si>
+  <si>
+    <t>Cabbage_Vegetable</t>
+  </si>
+  <si>
+    <t>Raddish_Vegetable</t>
+  </si>
+  <si>
+    <t>Guava_Fruit</t>
+  </si>
+  <si>
+    <t>Strawberry_Fruit</t>
   </si>
 </sst>
 </file>
@@ -450,13 +459,13 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
@@ -464,7 +473,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
@@ -496,7 +505,7 @@
         <v>6</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
@@ -504,7 +513,7 @@
         <v>7</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
@@ -512,7 +521,7 @@
         <v>8</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>2</v>
+        <v>13</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
@@ -520,7 +529,7 @@
         <v>9</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -528,7 +537,7 @@
         <v>10</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
@@ -536,7 +545,7 @@
         <v>108</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
@@ -544,32 +553,20 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>2</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1">
-        <v>-110</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>14</v>
-      </c>
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Timeunit to MS & Add message to assertion
</commit_message>
<xml_diff>
--- a/src/test/resources/product_catalog.xlsx
+++ b/src/test/resources/product_catalog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kapileson/Desktop/jmh-test-playground/src/test/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61C863D4-7F60-B244-A204-657CF98B7ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A8BA015-C40B-EC45-8286-DDEC162D5AAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="19880" xr2:uid="{8743DBB3-9E11-0445-A543-E7BF86D17E3C}"/>
   </bookViews>
@@ -456,10 +456,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2803A628-2C49-5745-8120-854287B0EC7F}">
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="176" workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -556,18 +556,6 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>